<commit_message>
scared of doing this
</commit_message>
<xml_diff>
--- a/Results/Main_Case/yearly_test.xlsx
+++ b/Results/Main_Case/yearly_test.xlsx
@@ -572,22 +572,26 @@
       <c r="L2" t="n">
         <v>0</v>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
-      <c r="P2" t="inlineStr"/>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q2" t="n">
-        <v>226.1684424189655</v>
+        <v>162.9941356354778</v>
       </c>
       <c r="R2" t="n">
-        <v>1198.506358155567</v>
+        <v>504.5149151680536</v>
       </c>
       <c r="S2" t="n">
-        <v>2515.403632457193</v>
+        <v>2807.261316242745</v>
       </c>
       <c r="T2" t="n">
         <v>3803910.933908072</v>
@@ -630,22 +634,26 @@
       <c r="L3" t="n">
         <v>0</v>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
       <c r="N3" t="n">
         <v>0</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
-      <c r="P3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
       <c r="Q3" t="n">
-        <v>224.9543686125816</v>
+        <v>228.7895586469373</v>
       </c>
       <c r="R3" t="n">
-        <v>3907.037677241527</v>
+        <v>2461.222272034012</v>
       </c>
       <c r="S3" t="n">
-        <v>2011.428003174287</v>
+        <v>2720.727186006326</v>
       </c>
       <c r="T3" t="n">
         <v>3803910.933908072</v>
@@ -688,22 +696,26 @@
       <c r="L4" t="n">
         <v>0</v>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
       <c r="N4" t="n">
         <v>0</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
       </c>
-      <c r="P4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
       <c r="Q4" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R4" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S4" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T4" t="n">
         <v>3803910.933908072</v>
@@ -711,7 +723,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>16571756.23995224</v>
@@ -746,22 +758,26 @@
       <c r="L5" t="n">
         <v>0</v>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
       </c>
-      <c r="P5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
       <c r="Q5" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R5" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S5" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T5" t="n">
         <v>3803910.933908072</v>
@@ -769,7 +785,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -804,22 +820,26 @@
       <c r="L6" t="n">
         <v>0</v>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
       </c>
-      <c r="P6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
       <c r="Q6" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R6" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S6" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T6" t="n">
         <v>3803910.933908072</v>
@@ -827,7 +847,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -862,22 +882,26 @@
       <c r="L7" t="n">
         <v>0</v>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
       </c>
-      <c r="P7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
       <c r="Q7" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R7" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S7" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T7" t="n">
         <v>3803910.933908072</v>
@@ -885,7 +909,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -920,22 +944,26 @@
       <c r="L8" t="n">
         <v>0</v>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
       <c r="N8" t="n">
         <v>0</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
-      <c r="P8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
       <c r="Q8" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R8" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S8" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T8" t="n">
         <v>3803910.933908072</v>
@@ -943,7 +971,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -978,22 +1006,26 @@
       <c r="L9" t="n">
         <v>0</v>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
       <c r="N9" t="n">
         <v>0</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
       </c>
-      <c r="P9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
       <c r="Q9" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R9" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S9" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T9" t="n">
         <v>3803910.933908072</v>
@@ -1001,7 +1033,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -1036,22 +1068,26 @@
       <c r="L10" t="n">
         <v>0</v>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
       </c>
-      <c r="P10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
       <c r="Q10" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R10" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S10" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T10" t="n">
         <v>3803910.933908072</v>
@@ -1059,7 +1095,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -1094,22 +1130,26 @@
       <c r="L11" t="n">
         <v>0</v>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
       <c r="N11" t="n">
         <v>0</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
-      <c r="P11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
       <c r="Q11" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R11" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S11" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T11" t="n">
         <v>3803910.933908072</v>
@@ -1117,7 +1157,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -1152,22 +1192,26 @@
       <c r="L12" t="n">
         <v>0</v>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
-      <c r="P12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
       <c r="Q12" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R12" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S12" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T12" t="n">
         <v>3803910.933908072</v>
@@ -1175,7 +1219,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -1210,22 +1254,26 @@
       <c r="L13" t="n">
         <v>0</v>
       </c>
-      <c r="M13" t="inlineStr"/>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
       <c r="N13" t="n">
         <v>0</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
-      <c r="P13" t="inlineStr"/>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
       <c r="Q13" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R13" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S13" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T13" t="n">
         <v>3803910.933908072</v>
@@ -1233,7 +1281,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -1268,22 +1316,26 @@
       <c r="L14" t="n">
         <v>0</v>
       </c>
-      <c r="M14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
         <v>0</v>
       </c>
-      <c r="P14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
       <c r="Q14" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R14" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S14" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T14" t="n">
         <v>3803910.933908072</v>
@@ -1291,7 +1343,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -1326,22 +1378,26 @@
       <c r="L15" t="n">
         <v>0</v>
       </c>
-      <c r="M15" t="inlineStr"/>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
       <c r="N15" t="n">
         <v>0</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
-      <c r="P15" t="inlineStr"/>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
       <c r="Q15" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R15" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S15" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T15" t="n">
         <v>3803910.933908072</v>
@@ -1349,7 +1405,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -1384,22 +1440,26 @@
       <c r="L16" t="n">
         <v>0</v>
       </c>
-      <c r="M16" t="inlineStr"/>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
       <c r="N16" t="n">
         <v>0</v>
       </c>
       <c r="O16" t="n">
         <v>0</v>
       </c>
-      <c r="P16" t="inlineStr"/>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
       <c r="Q16" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R16" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S16" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T16" t="n">
         <v>3803910.933908072</v>
@@ -1407,7 +1467,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -1442,22 +1502,26 @@
       <c r="L17" t="n">
         <v>0</v>
       </c>
-      <c r="M17" t="inlineStr"/>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
       <c r="N17" t="n">
         <v>0</v>
       </c>
       <c r="O17" t="n">
         <v>0</v>
       </c>
-      <c r="P17" t="inlineStr"/>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
       <c r="Q17" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R17" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S17" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T17" t="n">
         <v>3803910.933908072</v>
@@ -1465,7 +1529,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -1500,22 +1564,26 @@
       <c r="L18" t="n">
         <v>0</v>
       </c>
-      <c r="M18" t="inlineStr"/>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
       <c r="N18" t="n">
         <v>0</v>
       </c>
       <c r="O18" t="n">
         <v>0</v>
       </c>
-      <c r="P18" t="inlineStr"/>
+      <c r="P18" t="n">
+        <v>0</v>
+      </c>
       <c r="Q18" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R18" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S18" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T18" t="n">
         <v>3803910.933908072</v>
@@ -1523,7 +1591,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -1558,22 +1626,26 @@
       <c r="L19" t="n">
         <v>0</v>
       </c>
-      <c r="M19" t="inlineStr"/>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
       <c r="N19" t="n">
         <v>0</v>
       </c>
       <c r="O19" t="n">
         <v>0</v>
       </c>
-      <c r="P19" t="inlineStr"/>
+      <c r="P19" t="n">
+        <v>0</v>
+      </c>
       <c r="Q19" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R19" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S19" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T19" t="n">
         <v>3803910.933908072</v>
@@ -1581,7 +1653,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -1616,22 +1688,26 @@
       <c r="L20" t="n">
         <v>0</v>
       </c>
-      <c r="M20" t="inlineStr"/>
+      <c r="M20" t="n">
+        <v>0</v>
+      </c>
       <c r="N20" t="n">
         <v>0</v>
       </c>
       <c r="O20" t="n">
         <v>0</v>
       </c>
-      <c r="P20" t="inlineStr"/>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
       <c r="Q20" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R20" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S20" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T20" t="n">
         <v>3803910.933908072</v>
@@ -1639,7 +1715,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -1674,22 +1750,26 @@
       <c r="L21" t="n">
         <v>0</v>
       </c>
-      <c r="M21" t="inlineStr"/>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
       <c r="N21" t="n">
         <v>0</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
       </c>
-      <c r="P21" t="inlineStr"/>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
       <c r="Q21" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R21" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S21" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T21" t="n">
         <v>3803910.933908072</v>
@@ -1697,7 +1777,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -1732,22 +1812,26 @@
       <c r="L22" t="n">
         <v>0</v>
       </c>
-      <c r="M22" t="inlineStr"/>
+      <c r="M22" t="n">
+        <v>0</v>
+      </c>
       <c r="N22" t="n">
         <v>0</v>
       </c>
       <c r="O22" t="n">
         <v>0</v>
       </c>
-      <c r="P22" t="inlineStr"/>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
       <c r="Q22" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R22" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S22" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T22" t="n">
         <v>3803910.933908072</v>
@@ -1755,7 +1839,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
@@ -1790,22 +1874,26 @@
       <c r="L23" t="n">
         <v>0</v>
       </c>
-      <c r="M23" t="inlineStr"/>
+      <c r="M23" t="n">
+        <v>0</v>
+      </c>
       <c r="N23" t="n">
         <v>0</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
       </c>
-      <c r="P23" t="inlineStr"/>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
       <c r="Q23" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R23" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S23" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T23" t="n">
         <v>3803910.933908072</v>
@@ -1813,7 +1901,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -1848,22 +1936,26 @@
       <c r="L24" t="n">
         <v>0</v>
       </c>
-      <c r="M24" t="inlineStr"/>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
       <c r="N24" t="n">
         <v>0</v>
       </c>
       <c r="O24" t="n">
         <v>0</v>
       </c>
-      <c r="P24" t="inlineStr"/>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
       <c r="Q24" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R24" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S24" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T24" t="n">
         <v>3803910.933908072</v>
@@ -1871,7 +1963,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
@@ -1906,22 +1998,26 @@
       <c r="L25" t="n">
         <v>0</v>
       </c>
-      <c r="M25" t="inlineStr"/>
+      <c r="M25" t="n">
+        <v>0</v>
+      </c>
       <c r="N25" t="n">
         <v>0</v>
       </c>
       <c r="O25" t="n">
         <v>0</v>
       </c>
-      <c r="P25" t="inlineStr"/>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
       <c r="Q25" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R25" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S25" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T25" t="n">
         <v>3803910.933908072</v>
@@ -1929,7 +2025,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
@@ -1964,22 +2060,26 @@
       <c r="L26" t="n">
         <v>0</v>
       </c>
-      <c r="M26" t="inlineStr"/>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
       <c r="N26" t="n">
         <v>0</v>
       </c>
       <c r="O26" t="n">
         <v>0</v>
       </c>
-      <c r="P26" t="inlineStr"/>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
       <c r="Q26" t="n">
-        <v>222.7506899930604</v>
+        <v>219.4935176313175</v>
       </c>
       <c r="R26" t="n">
-        <v>7705.798801403123</v>
+        <v>5403.955159823739</v>
       </c>
       <c r="S26" t="n">
-        <v>1906.397634521698</v>
+        <v>2727.070397138864</v>
       </c>
       <c r="T26" t="n">
         <v>3803910.933908072</v>

</xml_diff>